<commit_message>
Actualización automática de ActualizacionObserver.xlsx - 2025-10-09 13:53:51
</commit_message>
<xml_diff>
--- a/ActualizacionObserver.xlsx
+++ b/ActualizacionObserver.xlsx
@@ -3281,10 +3281,10 @@
         <v>79400509048</v>
       </c>
       <c r="C178" t="n">
-        <v>6988.51</v>
+        <v>5808</v>
       </c>
       <c r="D178" t="n">
-        <v>10029</v>
+        <v>9589</v>
       </c>
     </row>
     <row r="179">
@@ -3524,7 +3524,7 @@
         <v>1329.92</v>
       </c>
       <c r="D193" t="n">
-        <v>3899</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="194">
@@ -3572,7 +3572,7 @@
         <v>1329.92</v>
       </c>
       <c r="D196" t="n">
-        <v>3899</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="197">

</xml_diff>

<commit_message>
Actualización automática de ActualizacionObserver.xlsx - 2025-10-09 13:57:40
</commit_message>
<xml_diff>
--- a/ActualizacionObserver.xlsx
+++ b/ActualizacionObserver.xlsx
@@ -3524,7 +3524,7 @@
         <v>1329.92</v>
       </c>
       <c r="D193" t="n">
-        <v>2199</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="194">
@@ -3572,7 +3572,7 @@
         <v>1329.92</v>
       </c>
       <c r="D196" t="n">
-        <v>2199</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="197">

</xml_diff>

<commit_message>
Actualización automática de ActualizacionObserver.xlsx - 2025-10-09 14:04:32
</commit_message>
<xml_diff>
--- a/ActualizacionObserver.xlsx
+++ b/ActualizacionObserver.xlsx
@@ -3524,7 +3524,7 @@
         <v>1329.92</v>
       </c>
       <c r="D193" t="n">
-        <v>3899</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="194">
@@ -3572,7 +3572,7 @@
         <v>1329.92</v>
       </c>
       <c r="D196" t="n">
-        <v>3899</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="197">

</xml_diff>